<commit_message>
Work on sensitivity analyses
</commit_message>
<xml_diff>
--- a/inst/models/checkimab/model.xlsx
+++ b/inst/models/checkimab/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrdnmdhl/Code/heRomod2/inst/models/checkimab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrdnmdhl/Code/openqaly packages/openqaly/inst/models/checkimab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3575A8F-2D14-BB49-BB12-AB8860DFA459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4920AE-CC98-E749-AD82-FE7ED02EF143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="194">
   <si>
     <t>timeframe</t>
   </si>
@@ -480,9 +480,6 @@
     <t>relapse_free_on_tx</t>
   </si>
   <si>
-    <t>ifelse(state_cycle &gt; 3, 0.2, 0.3)</t>
-  </si>
-  <si>
     <t>relapse_free_off_tx</t>
   </si>
   <si>
@@ -493,12 +490,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>0.01</t>
   </si>
   <si>
     <t>0.04</t>
@@ -2496,7 +2487,7 @@
   <dimension ref="A1:H569"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2542,7 +2533,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>73</v>
@@ -2564,7 +2555,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>73</v>
@@ -2586,7 +2577,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>73</v>
@@ -2608,7 +2599,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>73</v>
@@ -2738,7 +2729,7 @@
         <v>83</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>85</v>
@@ -2760,7 +2751,7 @@
         <v>83</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>85</v>
@@ -2782,7 +2773,7 @@
         <v>83</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>85</v>
@@ -2824,7 +2815,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>84</v>
@@ -2844,7 +2835,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>84</v>
@@ -2864,7 +2855,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>84</v>
@@ -2884,7 +2875,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>86</v>
@@ -2904,7 +2895,7 @@
         <v>44</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>86</v>
@@ -2924,7 +2915,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>86</v>
@@ -9015,7 +9006,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="G6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9052,13 +9043,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D2" t="s">
         <v>144</v>
@@ -9072,13 +9063,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D3" t="s">
         <v>144</v>
@@ -9092,13 +9083,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
         <v>144</v>
@@ -9112,13 +9103,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
         <v>144</v>
@@ -9127,18 +9118,18 @@
         <v>64</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D6" t="s">
         <v>144</v>
@@ -9147,18 +9138,18 @@
         <v>65</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
         <v>144</v>
@@ -9167,7 +9158,7 @@
         <v>28</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -9201,7 +9192,7 @@
         <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D9" t="s">
         <v>145</v>
@@ -9495,7 +9486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB106C64-597A-1343-B5D7-D61DA8E9983B}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -9512,27 +9503,27 @@
         <v>8</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="52" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D2">
         <v>100000</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -9549,21 +9540,21 @@
         <v>100000</v>
       </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -9575,11 +9566,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -9600,7 +9595,7 @@
         <v>149</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -9608,10 +9603,10 @@
         <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -9619,10 +9614,10 @@
         <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -9630,76 +9625,76 @@
         <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
         <v>151</v>
       </c>
-      <c r="B7" t="s">
-        <v>152</v>
-      </c>
       <c r="C7" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" t="s">
         <v>152</v>
       </c>
-      <c r="B10" t="s">
-        <v>153</v>
-      </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>